<commit_message>
Finally updated RUNY's name change
</commit_message>
<xml_diff>
--- a/2022MLR/Weekly Forecasts/Round_Finals.xlsx
+++ b/2022MLR/Weekly Forecasts/Round_Finals.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RugbyPredictifier\2022MLR\Weekly Forecasts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{9B9E1C74-C654-4C5C-9BD7-14FF2F6B4E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Finals" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>City</t>
   </si>
@@ -119,14 +112,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#0%"/>
     <numFmt numFmtId="167" formatCode="#0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,17 +210,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -235,14 +228,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -289,7 +274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,27 +306,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -373,24 +340,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -566,7 +515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -574,12 +523,9 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:61">
       <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
@@ -593,297 +539,369 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:61">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:61">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
-        <v>0.64299389891554681</v>
-      </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B3" s="5">
+        <v>0.6429938989155468</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:61">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
-        <v>0.95249277527710663</v>
-      </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>0.9526039301061378</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:61">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
-        <v>61.244704326431652</v>
-      </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>61.25185151412186</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:61">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>0.37239430000000001</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.62760570000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
+        <v>0.372542</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.627458</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
-        <v>23.048621399999998</v>
-      </c>
-      <c r="C7" s="5">
-        <v>27.148014799999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>23.0489246</v>
+      </c>
+      <c r="C7" s="7">
+        <v>27.149504</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <v>10</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="7">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:61">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="7">
         <v>13</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:61">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="7">
         <v>15</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="7">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:61">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="7">
         <v>17</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:61">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="7">
         <v>18</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:61">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="7">
         <v>19</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="7">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:61">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="7">
         <v>20</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="7">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:61">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="7">
         <v>21</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="7">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:61">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="7">
         <v>22</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="7">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="7">
         <v>24</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="7">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="7">
         <v>24</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="7">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="7">
         <v>25</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="7">
         <v>26</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="7">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="7">
         <v>27</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="7">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="7">
         <v>28</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="7">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="7">
         <v>29</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="7">
         <v>31</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="7">
         <v>33</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="7">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="7">
         <v>35</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="7">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
-        <v>5.9329600000000003E-2</v>
-      </c>
-      <c r="C27" s="4">
-        <v>7.6886399999999994E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="6">
+        <v>0.059333</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.07710939999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="4">
-        <v>0.22366320000000001</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0.18476719999999999</v>
+      <c r="B28" s="6">
+        <v>0.2235722</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.1848986</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="76">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>

</xml_diff>